<commit_message>
Fixed Census Data to match years and rerun results.
</commit_message>
<xml_diff>
--- a/Analysis/Output/Reg1_Rob.xlsx
+++ b/Analysis/Output/Reg1_Rob.xlsx
@@ -680,76 +680,76 @@
         <v>25</v>
       </c>
       <c r="B2" t="n">
-        <v>-4.41051166030872</v>
+        <v>-5.94837052197916</v>
       </c>
       <c r="C2" t="n">
-        <v>13.9690451552203</v>
+        <v>14.1318933565261</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.31573465554018</v>
+        <v>-0.42091815809183</v>
       </c>
       <c r="E2" t="n">
-        <v>0.757507516672876</v>
+        <v>0.681041478772298</v>
       </c>
       <c r="F2" t="n">
-        <v>-7.44687822593488</v>
+        <v>-7.15513469072085</v>
       </c>
       <c r="G2" t="n">
-        <v>16.9487463880073</v>
+        <v>16.9825146278408</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.439376344152755</v>
+        <v>-0.421323628892441</v>
       </c>
       <c r="I2" t="n">
-        <v>0.668761597753641</v>
+        <v>0.681513987397309</v>
       </c>
       <c r="J2" t="n">
-        <v>12.4273282995528</v>
+        <v>12.4198910391538</v>
       </c>
       <c r="K2" t="n">
-        <v>0.100521430965295</v>
+        <v>0.100649215449985</v>
       </c>
       <c r="L2" t="n">
-        <v>123.628644958738</v>
+        <v>123.397792855381</v>
       </c>
       <c r="M2" t="n">
-        <v>0.00000000000000298563785073631</v>
+        <v>0.0000000000000025532033581159</v>
       </c>
       <c r="N2" t="n">
-        <v>12.983450665119</v>
+        <v>12.962918021852</v>
       </c>
       <c r="O2" t="n">
-        <v>0.133444224575691</v>
+        <v>0.123401240501039</v>
       </c>
       <c r="P2" t="n">
-        <v>97.2949612948939</v>
+        <v>105.046902034529</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.00000000000000000000000640612496597317</v>
+        <v>0.00000000000000000000000145581971043194</v>
       </c>
       <c r="R2" t="n">
-        <v>13.4154169851349</v>
+        <v>13.413937283989</v>
       </c>
       <c r="S2" t="n">
-        <v>0.0477670139989049</v>
+        <v>0.0480100574899259</v>
       </c>
       <c r="T2" t="n">
-        <v>280.851069850052</v>
+        <v>279.398484094789</v>
       </c>
       <c r="U2" t="n">
-        <v>0.0000000000000000000000000000362347323611498</v>
+        <v>0.0000000000000000000000000000392945956459633</v>
       </c>
       <c r="V2" t="n">
-        <v>13.521464716208</v>
+        <v>13.5156461705516</v>
       </c>
       <c r="W2" t="n">
-        <v>0.0601419647661363</v>
+        <v>0.0601612997652174</v>
       </c>
       <c r="X2" t="n">
-        <v>224.825789592784</v>
+        <v>224.65681797596</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.000000000000000000000000000799293000687664</v>
+        <v>0.000000000000000000000000000827155546501598</v>
       </c>
     </row>
     <row r="3">
@@ -757,76 +757,76 @@
         <v>26</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0212627811009832</v>
+        <v>0.0204399640349742</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00917121738921548</v>
+        <v>0.00973821019622369</v>
       </c>
       <c r="D3" t="n">
-        <v>2.31842515542008</v>
+        <v>2.09894463388153</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0358596280876008</v>
+        <v>0.0542011248257915</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0192367304054154</v>
+        <v>0.0188344670804024</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0108466294506203</v>
+        <v>0.011009014366803</v>
       </c>
       <c r="H3" t="n">
-        <v>1.77352148821819</v>
+        <v>1.71082228189261</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0976181288274367</v>
+        <v>0.10889932328404</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0216527676250705</v>
+        <v>0.0211476946893071</v>
       </c>
       <c r="K3" t="n">
-        <v>0.010938888454964</v>
+        <v>0.0111324480195603</v>
       </c>
       <c r="L3" t="n">
-        <v>1.97943033373238</v>
+        <v>1.89964459318826</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0675244889336755</v>
+        <v>0.0780166838431823</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0147517269161338</v>
+        <v>0.0144259384551829</v>
       </c>
       <c r="O3" t="n">
-        <v>0.0112684001778345</v>
+        <v>0.0114135212714287</v>
       </c>
       <c r="P3" t="n">
-        <v>1.309123449942</v>
+        <v>1.26393407539312</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.211324261401837</v>
+        <v>0.226650759724293</v>
       </c>
       <c r="R3" t="n">
-        <v>0.0376445744252488</v>
+        <v>0.0376616650769112</v>
       </c>
       <c r="S3" t="n">
-        <v>0.023249924154927</v>
+        <v>0.0232069853174775</v>
       </c>
       <c r="T3" t="n">
-        <v>1.61912676249618</v>
+        <v>1.62285900394601</v>
       </c>
       <c r="U3" t="n">
-        <v>0.127454473389872</v>
+        <v>0.12664961915562</v>
       </c>
       <c r="V3" t="n">
-        <v>0.0721134992724978</v>
+        <v>0.0778977571703646</v>
       </c>
       <c r="W3" t="n">
-        <v>0.0243690620716396</v>
+        <v>0.0222801837321574</v>
       </c>
       <c r="X3" t="n">
-        <v>2.95922342273577</v>
+        <v>3.49627983803084</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.00952910205254688</v>
+        <v>0.00313730601991328</v>
       </c>
     </row>
     <row r="4">
@@ -834,64 +834,64 @@
         <v>27</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0000631835203418442</v>
+        <v>0.0000884335991475713</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0000705720072373161</v>
+        <v>0.0000724306448803328</v>
       </c>
       <c r="D4" t="n">
-        <v>0.895305700025985</v>
+        <v>1.220941761511</v>
       </c>
       <c r="E4" t="n">
-        <v>0.390499740583156</v>
+        <v>0.248337425293832</v>
       </c>
       <c r="F4" t="n">
-        <v>0.000110660852378379</v>
+        <v>0.000125041950572184</v>
       </c>
       <c r="G4" t="n">
-        <v>0.000069097995281951</v>
+        <v>0.0000734696025962464</v>
       </c>
       <c r="H4" t="n">
-        <v>1.60150597606823</v>
+        <v>1.7019549058861</v>
       </c>
       <c r="I4" t="n">
-        <v>0.138411943748573</v>
+        <v>0.117390092321256</v>
       </c>
       <c r="J4" t="n">
-        <v>0.000163202209644543</v>
+        <v>0.000182406282608051</v>
       </c>
       <c r="K4" t="n">
-        <v>0.000107974341152494</v>
+        <v>0.000111898837269214</v>
       </c>
       <c r="L4" t="n">
-        <v>1.51149067364115</v>
+        <v>1.63009989254138</v>
       </c>
       <c r="M4" t="n">
-        <v>0.159613292082012</v>
+        <v>0.131861145760818</v>
       </c>
       <c r="N4" t="n">
-        <v>0.000111371496421769</v>
+        <v>0.000140494534967041</v>
       </c>
       <c r="O4" t="n">
-        <v>0.000160305194548291</v>
+        <v>0.000162702499144498</v>
       </c>
       <c r="P4" t="n">
-        <v>0.69474664707898</v>
+        <v>0.86350569724357</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.502185389206057</v>
+        <v>0.406784597112143</v>
       </c>
       <c r="R4" t="n">
-        <v>0.00101208937615819</v>
+        <v>0.00103063166600527</v>
       </c>
       <c r="S4" t="n">
-        <v>0.000279706599104503</v>
+        <v>0.000279088636876374</v>
       </c>
       <c r="T4" t="n">
-        <v>3.61839648902976</v>
+        <v>3.69284710957902</v>
       </c>
       <c r="U4" t="n">
-        <v>0.0043708648498302</v>
+        <v>0.00381654324955162</v>
       </c>
       <c r="V4"/>
       <c r="W4"/>
@@ -903,64 +903,64 @@
         <v>28</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0476049900888517</v>
+        <v>0.0358642931027096</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0154991130270735</v>
+        <v>0.0112260903258733</v>
       </c>
       <c r="D5" t="n">
-        <v>3.07146544487393</v>
+        <v>3.19472693178421</v>
       </c>
       <c r="E5" t="n">
-        <v>0.007718490591877</v>
+        <v>0.005993481992883</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0456917305136211</v>
+        <v>0.0395537318087666</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0141354563057064</v>
+        <v>0.0110773913291392</v>
       </c>
       <c r="H5" t="n">
-        <v>3.23241991807336</v>
+        <v>3.57067206831631</v>
       </c>
       <c r="I5" t="n">
-        <v>0.00555391529005692</v>
+        <v>0.00276723645231184</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0395561740801495</v>
+        <v>0.0318774283418323</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0173326778605249</v>
+        <v>0.0133994880858563</v>
       </c>
       <c r="L5" t="n">
-        <v>2.28217326823102</v>
+        <v>2.37900344681677</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0374251620603809</v>
+        <v>0.0309919309822563</v>
       </c>
       <c r="N5" t="n">
-        <v>0.0424953741702552</v>
+        <v>0.0310062155784838</v>
       </c>
       <c r="O5" t="n">
-        <v>0.0222054281618985</v>
+        <v>0.0154438879215177</v>
       </c>
       <c r="P5" t="n">
-        <v>1.91373811215996</v>
+        <v>2.00766903619414</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.0748438875260405</v>
+        <v>0.0629528249560103</v>
       </c>
       <c r="R5" t="n">
-        <v>0.0801259791288333</v>
+        <v>0.0611078798154861</v>
       </c>
       <c r="S5" t="n">
-        <v>0.0296577802832034</v>
+        <v>0.0150212802872638</v>
       </c>
       <c r="T5" t="n">
-        <v>2.70168496643063</v>
+        <v>4.06808731658501</v>
       </c>
       <c r="U5" t="n">
-        <v>0.0163677602705712</v>
+        <v>0.00100106935434916</v>
       </c>
       <c r="V5"/>
       <c r="W5"/>
@@ -972,64 +972,64 @@
         <v>29</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0549269141266349</v>
+        <v>0.0444910342196231</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0155070898561772</v>
+        <v>0.016843943105796</v>
       </c>
       <c r="D6" t="n">
-        <v>3.5420517089965</v>
+        <v>2.64136692579505</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00299418441559345</v>
+        <v>0.0185740420898688</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0542164498884107</v>
+        <v>0.0519570775195699</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0157597857242138</v>
+        <v>0.0143079590270308</v>
       </c>
       <c r="H6" t="n">
-        <v>3.44017684232285</v>
+        <v>3.63134094956604</v>
       </c>
       <c r="I6" t="n">
-        <v>0.00368665412431952</v>
+        <v>0.00249524090748271</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0435049058515174</v>
+        <v>0.0410940336010326</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0178347598945875</v>
+        <v>0.0163829688242675</v>
       </c>
       <c r="L6" t="n">
-        <v>2.43933229876116</v>
+        <v>2.50833863152821</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0277360578207412</v>
+        <v>0.0242227734081765</v>
       </c>
       <c r="N6" t="n">
-        <v>0.042640006161358</v>
+        <v>0.040517629454688</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0198933088360175</v>
+        <v>0.0186786448733459</v>
       </c>
       <c r="P6" t="n">
-        <v>2.1434345846055</v>
+        <v>2.16919534202965</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.0490414845659469</v>
+        <v>0.0467113787614877</v>
       </c>
       <c r="R6" t="n">
-        <v>0.0708171644968718</v>
+        <v>0.0679046894028279</v>
       </c>
       <c r="S6" t="n">
-        <v>0.0176524003398193</v>
+        <v>0.016051533498873</v>
       </c>
       <c r="T6" t="n">
-        <v>4.01175835204272</v>
+        <v>4.2304175739717</v>
       </c>
       <c r="U6" t="n">
-        <v>0.00115342057788702</v>
+        <v>0.00074285406588074</v>
       </c>
       <c r="V6"/>
       <c r="W6"/>
@@ -1041,64 +1041,64 @@
         <v>30</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0402957498233153</v>
+        <v>0.0333359191604069</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0162702878023418</v>
+        <v>0.0178131545423672</v>
       </c>
       <c r="D7" t="n">
-        <v>2.47664640680268</v>
+        <v>1.87142143078139</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0255068421660168</v>
+        <v>0.0806403065310271</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0382964799571688</v>
+        <v>0.0382638810219322</v>
       </c>
       <c r="G7" t="n">
-        <v>0.014871353658089</v>
+        <v>0.0148358098978071</v>
       </c>
       <c r="H7" t="n">
-        <v>2.57518453515751</v>
+        <v>2.57915687013407</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0209776454882396</v>
+        <v>0.0208124023280811</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0264292836121805</v>
+        <v>0.0264275165180369</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0161544040377943</v>
+        <v>0.0161289608703151</v>
       </c>
       <c r="L7" t="n">
-        <v>1.6360420075137</v>
+        <v>1.63851327624434</v>
       </c>
       <c r="M7" t="n">
-        <v>0.122411372873682</v>
+        <v>0.121891665920712</v>
       </c>
       <c r="N7" t="n">
-        <v>0.0324334363478613</v>
+        <v>0.0328530466287318</v>
       </c>
       <c r="O7" t="n">
-        <v>0.0184480872628316</v>
+        <v>0.018743771232389</v>
       </c>
       <c r="P7" t="n">
-        <v>1.75809209300558</v>
+        <v>1.75274475031802</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.0988925461994249</v>
+        <v>0.0998345038247508</v>
       </c>
       <c r="R7" t="n">
-        <v>0.0643839348960837</v>
+        <v>0.0650046990884817</v>
       </c>
       <c r="S7" t="n">
-        <v>0.0135466814473381</v>
+        <v>0.0139423750299691</v>
       </c>
       <c r="T7" t="n">
-        <v>4.75274591392528</v>
+        <v>4.66238348550762</v>
       </c>
       <c r="U7" t="n">
-        <v>0.000249797583473876</v>
+        <v>0.00029885326184373</v>
       </c>
       <c r="V7"/>
       <c r="W7"/>
@@ -1110,64 +1110,64 @@
         <v>31</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0192706173742921</v>
+        <v>0.0143173953572881</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0183572581476116</v>
+        <v>0.0227623681779905</v>
       </c>
       <c r="D8" t="n">
-        <v>1.04975466484897</v>
+        <v>0.628994103132553</v>
       </c>
       <c r="E8" t="n">
-        <v>0.311563033119138</v>
+        <v>0.53943902234932</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0213451128853614</v>
+        <v>0.02144174219426</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0187157030720703</v>
+        <v>0.0187828513350152</v>
       </c>
       <c r="H8" t="n">
-        <v>1.14049217404047</v>
+        <v>1.1415594901871</v>
       </c>
       <c r="I8" t="n">
-        <v>0.273163632895891</v>
+        <v>0.272734257043736</v>
       </c>
       <c r="J8" t="n">
-        <v>0.00663631967274799</v>
+        <v>0.00672698752513459</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0186461278437481</v>
+        <v>0.0187167175019084</v>
       </c>
       <c r="L8" t="n">
-        <v>0.355908729595732</v>
+        <v>0.359410645827651</v>
       </c>
       <c r="M8" t="n">
-        <v>0.727199835994674</v>
+        <v>0.724635980919947</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0185626811484565</v>
+        <v>0.0188450979787398</v>
       </c>
       <c r="O8" t="n">
-        <v>0.0236617315188483</v>
+        <v>0.0237993836168521</v>
       </c>
       <c r="P8" t="n">
-        <v>0.784502230264507</v>
+        <v>0.791831346648647</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.445787720169409</v>
+        <v>0.441639589027681</v>
       </c>
       <c r="R8" t="n">
-        <v>0.0556229201432893</v>
+        <v>0.0560921937848587</v>
       </c>
       <c r="S8" t="n">
-        <v>0.0303469691088975</v>
+        <v>0.0305490151383352</v>
       </c>
       <c r="T8" t="n">
-        <v>1.83289869718756</v>
+        <v>1.83613754914377</v>
       </c>
       <c r="U8" t="n">
-        <v>0.0881210425490132</v>
+        <v>0.0876165799384052</v>
       </c>
       <c r="V8"/>
       <c r="W8"/>
@@ -1179,64 +1179,64 @@
         <v>32</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0927278029341493</v>
+        <v>0.0860908975556521</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0220542979607206</v>
+        <v>0.0274469505247849</v>
       </c>
       <c r="D9" t="n">
-        <v>4.20452299589407</v>
+        <v>3.13662887532482</v>
       </c>
       <c r="E9" t="n">
-        <v>0.000835122235528828</v>
+        <v>0.00707640633177169</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0942405705719332</v>
+        <v>0.0950179913862653</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0223875660882753</v>
+        <v>0.0225405953447223</v>
       </c>
       <c r="H9" t="n">
-        <v>4.20950496361856</v>
+        <v>4.21541622717224</v>
       </c>
       <c r="I9" t="n">
-        <v>0.000826894366624237</v>
+        <v>0.000817397790143123</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0790020404066131</v>
+        <v>0.0799968301549038</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0215690694006324</v>
+        <v>0.0218580589851967</v>
       </c>
       <c r="L9" t="n">
-        <v>3.66274682227582</v>
+        <v>3.65983229385013</v>
       </c>
       <c r="M9" t="n">
-        <v>0.00245817237376426</v>
+        <v>0.00247277958870342</v>
       </c>
       <c r="N9" t="n">
-        <v>0.0862850808661883</v>
+        <v>0.0873324845658613</v>
       </c>
       <c r="O9" t="n">
-        <v>0.0285879610438777</v>
+        <v>0.0289894124302917</v>
       </c>
       <c r="P9" t="n">
-        <v>3.01823137137186</v>
+        <v>3.0125648381409</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.00899368225486192</v>
+        <v>0.00909669985312407</v>
       </c>
       <c r="R9" t="n">
-        <v>0.109504423387811</v>
+        <v>0.110355962280246</v>
       </c>
       <c r="S9" t="n">
-        <v>0.0516407427807707</v>
+        <v>0.0517583629251865</v>
       </c>
       <c r="T9" t="n">
-        <v>2.12050442133816</v>
+        <v>2.13213780427636</v>
       </c>
       <c r="U9" t="n">
-        <v>0.0518487656983089</v>
+        <v>0.0507345344668833</v>
       </c>
       <c r="V9"/>
       <c r="W9"/>
@@ -1248,64 +1248,64 @@
         <v>33</v>
       </c>
       <c r="B10" t="n">
-        <v>0.135002876153203</v>
+        <v>0.128292025300926</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0250655319005916</v>
+        <v>0.0299987542974196</v>
       </c>
       <c r="D10" t="n">
-        <v>5.38599686169103</v>
+        <v>4.27657842152338</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0000869848984674143</v>
+        <v>0.000719968531586593</v>
       </c>
       <c r="F10" t="n">
-        <v>0.136648822591281</v>
+        <v>0.137362680214233</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0254561989223594</v>
+        <v>0.0256425254118175</v>
       </c>
       <c r="H10" t="n">
-        <v>5.36799790919515</v>
+        <v>5.35683120161511</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0000898954954332446</v>
+        <v>0.0000917877837179926</v>
       </c>
       <c r="J10" t="n">
-        <v>0.11365190007344</v>
+        <v>0.114514430951914</v>
       </c>
       <c r="K10" t="n">
-        <v>0.0251578139161353</v>
+        <v>0.0255171178923335</v>
       </c>
       <c r="L10" t="n">
-        <v>4.51755865800996</v>
+        <v>4.48774941727722</v>
       </c>
       <c r="M10" t="n">
-        <v>0.000450596570055729</v>
+        <v>0.000477593960660498</v>
       </c>
       <c r="N10" t="n">
-        <v>0.121610775565862</v>
+        <v>0.122459754647659</v>
       </c>
       <c r="O10" t="n">
-        <v>0.033894788346449</v>
+        <v>0.0342598626877028</v>
       </c>
       <c r="P10" t="n">
-        <v>3.58789010047329</v>
+        <v>3.57443798779772</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.0028528118590987</v>
+        <v>0.00293122835298237</v>
       </c>
       <c r="R10" t="n">
-        <v>0.125545603388594</v>
+        <v>0.126477626956549</v>
       </c>
       <c r="S10" t="n">
-        <v>0.0554633912078304</v>
+        <v>0.0555606559476699</v>
       </c>
       <c r="T10" t="n">
-        <v>2.26357603915985</v>
+        <v>2.27638829670536</v>
       </c>
       <c r="U10" t="n">
-        <v>0.0395688221424852</v>
+        <v>0.0386159636182684</v>
       </c>
       <c r="V10"/>
       <c r="W10"/>
@@ -1317,64 +1317,64 @@
         <v>34</v>
       </c>
       <c r="B11" t="n">
-        <v>0.101137137558345</v>
+        <v>0.0963955176264928</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0285223205078244</v>
+        <v>0.0348697225387785</v>
       </c>
       <c r="D11" t="n">
-        <v>3.54589443487251</v>
+        <v>2.76444750942</v>
       </c>
       <c r="E11" t="n">
-        <v>0.00284609079107257</v>
+        <v>0.0142284042935338</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0917271486061232</v>
+        <v>0.0932542678063548</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0309654342093279</v>
+        <v>0.0315265661662991</v>
       </c>
       <c r="H11" t="n">
-        <v>2.96224325439918</v>
+        <v>2.95795829188783</v>
       </c>
       <c r="I11" t="n">
-        <v>0.00950757446484109</v>
+        <v>0.00959134734282942</v>
       </c>
       <c r="J11" t="n">
-        <v>0.0572352994278458</v>
+        <v>0.0591497287320697</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0391722604067225</v>
+        <v>0.0395713314666739</v>
       </c>
       <c r="L11" t="n">
-        <v>1.46111811862722</v>
+        <v>1.49476215582699</v>
       </c>
       <c r="M11" t="n">
-        <v>0.164169203744852</v>
+        <v>0.155267786141361</v>
       </c>
       <c r="N11" t="n">
-        <v>0.125312586325559</v>
+        <v>0.123393931508497</v>
       </c>
       <c r="O11" t="n">
-        <v>0.0460003377418464</v>
+        <v>0.0448735401275637</v>
       </c>
       <c r="P11" t="n">
-        <v>2.72416665783658</v>
+        <v>2.74981495014034</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.0154835931366695</v>
+        <v>0.014700886277713</v>
       </c>
       <c r="R11" t="n">
-        <v>0.446635318382647</v>
+        <v>0.447198744437208</v>
       </c>
       <c r="S11" t="n">
-        <v>0.0677205288717356</v>
+        <v>0.0678457520364951</v>
       </c>
       <c r="T11" t="n">
-        <v>6.59527215489686</v>
+        <v>6.59140375062324</v>
       </c>
       <c r="U11" t="n">
-        <v>0.0000077324322902568</v>
+        <v>0.00000778516541551004</v>
       </c>
       <c r="V11"/>
       <c r="W11"/>
@@ -1386,52 +1386,52 @@
         <v>35</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0251160166624746</v>
+        <v>0.0242590220461043</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0222919584520449</v>
+        <v>0.022647513203914</v>
       </c>
       <c r="D12" t="n">
-        <v>1.12668506522228</v>
+        <v>1.07115610564748</v>
       </c>
       <c r="E12" t="n">
-        <v>0.274317891499372</v>
+        <v>0.297912849382025</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0131891700415523</v>
+        <v>0.0129843345321531</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0240526843480805</v>
+        <v>0.0240682280395322</v>
       </c>
       <c r="H12" t="n">
-        <v>0.54834503503576</v>
+        <v>0.539480285413046</v>
       </c>
       <c r="I12" t="n">
-        <v>0.590047560818029</v>
+        <v>0.596026463161498</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.0140874117538545</v>
+        <v>-0.0142870965826194</v>
       </c>
       <c r="K12" t="n">
-        <v>0.0238456858207894</v>
+        <v>0.0238374939310731</v>
       </c>
       <c r="L12" t="n">
-        <v>-0.590774023432477</v>
+        <v>-0.599353968329516</v>
       </c>
       <c r="M12" t="n">
-        <v>0.561870913624964</v>
+        <v>0.556259406411888</v>
       </c>
       <c r="N12" t="n">
-        <v>0.033876841218653</v>
+        <v>0.0345495074235986</v>
       </c>
       <c r="O12" t="n">
-        <v>0.0189403806548456</v>
+        <v>0.0189965626488874</v>
       </c>
       <c r="P12" t="n">
-        <v>1.78860403262202</v>
+        <v>1.81872415879523</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.0905727307308678</v>
+        <v>0.0856793387626332</v>
       </c>
       <c r="R12"/>
       <c r="S12"/>
@@ -1447,52 +1447,52 @@
         <v>36</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0518325593379722</v>
+        <v>0.0543515355492346</v>
       </c>
       <c r="C13" t="n">
-        <v>0.016390208920876</v>
+        <v>0.0163970544315804</v>
       </c>
       <c r="D13" t="n">
-        <v>3.16240992339967</v>
+        <v>3.31471336977174</v>
       </c>
       <c r="E13" t="n">
-        <v>0.00540341649274735</v>
+        <v>0.00387614985634926</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0614707527618119</v>
+        <v>0.0612334299773935</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0188745248383359</v>
+        <v>0.0188425282817456</v>
       </c>
       <c r="H13" t="n">
-        <v>3.25681061050921</v>
+        <v>3.24974595032004</v>
       </c>
       <c r="I13" t="n">
-        <v>0.00438511104650181</v>
+        <v>0.00446744685919089</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0902118862441423</v>
+        <v>0.0905010584383866</v>
       </c>
       <c r="K13" t="n">
-        <v>0.0266203548166633</v>
+        <v>0.0265314813559563</v>
       </c>
       <c r="L13" t="n">
-        <v>3.3888310980616</v>
+        <v>3.41108199818134</v>
       </c>
       <c r="M13" t="n">
-        <v>0.00329895654105954</v>
+        <v>0.00315104876877141</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0899572489819525</v>
+        <v>0.0903570424817304</v>
       </c>
       <c r="O13" t="n">
-        <v>0.0283699969842776</v>
+        <v>0.0285847118911764</v>
       </c>
       <c r="P13" t="n">
-        <v>3.17085860219886</v>
+        <v>3.16102687428598</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.00527882327160901</v>
+        <v>0.00540890101893272</v>
       </c>
       <c r="R13"/>
       <c r="S13"/>
@@ -1508,52 +1508,52 @@
         <v>37</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0560826941033493</v>
+        <v>0.0568205393248291</v>
       </c>
       <c r="C14" t="n">
-        <v>0.00995165545826493</v>
+        <v>0.00900998973172828</v>
       </c>
       <c r="D14" t="n">
-        <v>5.63551404472833</v>
+        <v>6.30639334967699</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0000449648086638712</v>
+        <v>0.0000133648115610369</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0580215254754796</v>
+        <v>0.0567242391674869</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0101284980868926</v>
+        <v>0.0093228541356087</v>
       </c>
       <c r="H14" t="n">
-        <v>5.72854188031746</v>
+        <v>6.08442847462649</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0000377517177766147</v>
+        <v>0.0000199997277443872</v>
       </c>
       <c r="J14" t="n">
-        <v>0.0479762269898742</v>
+        <v>0.0471526026788843</v>
       </c>
       <c r="K14" t="n">
-        <v>0.0145696967466348</v>
+        <v>0.0142411438925342</v>
       </c>
       <c r="L14" t="n">
-        <v>3.29287752684046</v>
+        <v>3.3110123059429</v>
       </c>
       <c r="M14" t="n">
-        <v>0.00487627903510496</v>
+        <v>0.00472038006519061</v>
       </c>
       <c r="N14" t="n">
-        <v>0.0634558937372855</v>
+        <v>0.0637092049757066</v>
       </c>
       <c r="O14" t="n">
-        <v>0.0189286376241463</v>
+        <v>0.0191000807457178</v>
       </c>
       <c r="P14" t="n">
-        <v>3.35237511527707</v>
+        <v>3.33554636882832</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.00437127690556253</v>
+        <v>0.00454314301393937</v>
       </c>
       <c r="R14"/>
       <c r="S14"/>
@@ -1569,52 +1569,52 @@
         <v>38</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.0966001853876958</v>
+        <v>-0.0932691258043367</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0318611184569449</v>
+        <v>0.0294654387702071</v>
       </c>
       <c r="D15" t="n">
-        <v>-3.03191444827134</v>
+        <v>-3.16537372926014</v>
       </c>
       <c r="E15" t="n">
-        <v>0.00858945096694338</v>
+        <v>0.00658084967376172</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.0989917009906115</v>
+        <v>-0.0968607270263143</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0300355750850825</v>
+        <v>0.0289553665861358</v>
       </c>
       <c r="H15" t="n">
-        <v>-3.29581506963643</v>
+        <v>-3.34517357043901</v>
       </c>
       <c r="I15" t="n">
-        <v>0.00509571244055356</v>
+        <v>0.00461804000837594</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.108299394239513</v>
+        <v>-0.105699613515534</v>
       </c>
       <c r="K15" t="n">
-        <v>0.0348202149493408</v>
+        <v>0.0334866275208141</v>
       </c>
       <c r="L15" t="n">
-        <v>-3.11024485050066</v>
+        <v>-3.15647233958794</v>
       </c>
       <c r="M15" t="n">
-        <v>0.00733259099423263</v>
+        <v>0.00668606347552282</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.186199504689483</v>
+        <v>-0.181647065362314</v>
       </c>
       <c r="O15" t="n">
-        <v>0.047409213457807</v>
+        <v>0.0444792221394089</v>
       </c>
       <c r="P15" t="n">
-        <v>-3.92749617867413</v>
+        <v>-4.08386335518609</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.00129948903938036</v>
+        <v>0.00094346224071855</v>
       </c>
       <c r="R15"/>
       <c r="S15"/>
@@ -1630,52 +1630,52 @@
         <v>39</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.0494557504825147</v>
+        <v>-0.0545935090709218</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0113487139549682</v>
+        <v>0.0100814330724225</v>
       </c>
       <c r="D16" t="n">
-        <v>-4.35782862082483</v>
+        <v>-5.41525283942625</v>
       </c>
       <c r="E16" t="n">
-        <v>0.000889526573671966</v>
+        <v>0.000144744696675341</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.0544461607337399</v>
+        <v>-0.0561178491952584</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0123689779106708</v>
+        <v>0.0124449171749107</v>
       </c>
       <c r="H16" t="n">
-        <v>-4.40183183501111</v>
+        <v>-4.50929872867241</v>
       </c>
       <c r="I16" t="n">
-        <v>0.000817627100214422</v>
+        <v>0.00067354613732484</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.0299125725176342</v>
+        <v>-0.0321112806992923</v>
       </c>
       <c r="K16" t="n">
-        <v>0.0135604554370431</v>
+        <v>0.0134630241101246</v>
       </c>
       <c r="L16" t="n">
-        <v>-2.2058678380316</v>
+        <v>-2.38514619275944</v>
       </c>
       <c r="M16" t="n">
-        <v>0.0471092953879879</v>
+        <v>0.0339449943839965</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.0794739317653222</v>
+        <v>-0.0867679113371133</v>
       </c>
       <c r="O16" t="n">
-        <v>0.0584977576205419</v>
+        <v>0.0572698672634813</v>
       </c>
       <c r="P16" t="n">
-        <v>-1.35858082425734</v>
+        <v>-1.51507093491103</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.194588217901699</v>
+        <v>0.150786346990278</v>
       </c>
       <c r="R16"/>
       <c r="S16"/>
@@ -1691,52 +1691,52 @@
         <v>40</v>
       </c>
       <c r="B17" t="n">
-        <v>0.000207445294243177</v>
+        <v>0.000206191632950542</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0000188772628437385</v>
+        <v>0.0000185370875037982</v>
       </c>
       <c r="D17" t="n">
-        <v>10.9891617211859</v>
+        <v>11.1231946716707</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0000000171859037989871</v>
+        <v>0.0000000145875202628468</v>
       </c>
       <c r="F17" t="n">
-        <v>0.000228983150459994</v>
+        <v>0.000227730152200189</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0000220898384550087</v>
+        <v>0.0000215412736938724</v>
       </c>
       <c r="H17" t="n">
-        <v>10.3659947955877</v>
+        <v>10.5718053368854</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0000000396969311621397</v>
+        <v>0.0000000302502725524888</v>
       </c>
       <c r="J17" t="n">
-        <v>0.000286685180312806</v>
+        <v>0.000284814784437634</v>
       </c>
       <c r="K17" t="n">
-        <v>0.0000258213894954249</v>
+        <v>0.0000250146405616656</v>
       </c>
       <c r="L17" t="n">
-        <v>11.1026240614821</v>
+        <v>11.3859235248859</v>
       </c>
       <c r="M17" t="n">
-        <v>0.0000000139428335900645</v>
+        <v>0.00000000981267819819305</v>
       </c>
       <c r="N17" t="n">
-        <v>0.000333691796262075</v>
+        <v>0.000331571943098994</v>
       </c>
       <c r="O17" t="n">
-        <v>0.0000194780931908509</v>
+        <v>0.0000187710497638864</v>
       </c>
       <c r="P17" t="n">
-        <v>17.1316459466789</v>
+        <v>17.6640063965365</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.000000000030009297388845</v>
+        <v>0.0000000000190110403783942</v>
       </c>
       <c r="R17"/>
       <c r="S17"/>
@@ -1752,52 +1752,52 @@
         <v>41</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.0146315378799845</v>
+        <v>-0.0140703514744464</v>
       </c>
       <c r="C18" t="n">
-        <v>0.00495324109546783</v>
+        <v>0.00451823679380796</v>
       </c>
       <c r="D18" t="n">
-        <v>-2.95393210182564</v>
+        <v>-3.11412440661126</v>
       </c>
       <c r="E18" t="n">
-        <v>0.00992355541956216</v>
+        <v>0.00694497776959558</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.0149351494495747</v>
+        <v>-0.0143455903431694</v>
       </c>
       <c r="G18" t="n">
-        <v>0.00426899309673741</v>
+        <v>0.00398927533118866</v>
       </c>
       <c r="H18" t="n">
-        <v>-3.49851806061456</v>
+        <v>-3.5960391680699</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0032587596477631</v>
+        <v>0.00252777930875257</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.010757086457617</v>
+        <v>-0.0100687642924833</v>
       </c>
       <c r="K18" t="n">
-        <v>0.00514375820831691</v>
+        <v>0.00478704008690211</v>
       </c>
       <c r="L18" t="n">
-        <v>-2.09128929120811</v>
+        <v>-2.10333820266779</v>
       </c>
       <c r="M18" t="n">
-        <v>0.0539613949018979</v>
+        <v>0.0521988764140566</v>
       </c>
       <c r="N18" t="n">
-        <v>-0.0167368293819436</v>
+        <v>-0.0156891928958192</v>
       </c>
       <c r="O18" t="n">
-        <v>0.00584061796027757</v>
+        <v>0.0052120679261042</v>
       </c>
       <c r="P18" t="n">
-        <v>-2.8655922191405</v>
+        <v>-3.01016662066917</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.0122220771490008</v>
+        <v>0.00874210591926901</v>
       </c>
       <c r="R18"/>
       <c r="S18"/>
@@ -1813,52 +1813,52 @@
         <v>42</v>
       </c>
       <c r="B19" t="n">
-        <v>0.154148578312398</v>
+        <v>0.148493523788512</v>
       </c>
       <c r="C19" t="n">
-        <v>0.048424958449036</v>
+        <v>0.043947316506553</v>
       </c>
       <c r="D19" t="n">
-        <v>3.18324647556753</v>
+        <v>3.37889854472388</v>
       </c>
       <c r="E19" t="n">
-        <v>0.00626376724295541</v>
+        <v>0.00415656586325912</v>
       </c>
       <c r="F19" t="n">
-        <v>0.162491020492098</v>
+        <v>0.155993271791955</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0439231010579386</v>
+        <v>0.0408545955521653</v>
       </c>
       <c r="H19" t="n">
-        <v>3.69944326739949</v>
+        <v>3.8182551970873</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0021481439472191</v>
+        <v>0.00164952815475032</v>
       </c>
       <c r="J19" t="n">
-        <v>0.153713977237893</v>
+        <v>0.14627509519359</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0504599567261051</v>
+        <v>0.0466157029867595</v>
       </c>
       <c r="L19" t="n">
-        <v>3.04625662031871</v>
+        <v>3.13789315233834</v>
       </c>
       <c r="M19" t="n">
-        <v>0.00824600508619259</v>
+        <v>0.00678080241930464</v>
       </c>
       <c r="N19" t="n">
-        <v>0.207157198165736</v>
+        <v>0.196312127945961</v>
       </c>
       <c r="O19" t="n">
-        <v>0.0517414878785205</v>
+        <v>0.0455819061654352</v>
       </c>
       <c r="P19" t="n">
-        <v>4.0036961954419</v>
+        <v>4.30679943996779</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.00116932773301348</v>
+        <v>0.00061738471862054</v>
       </c>
       <c r="R19"/>
       <c r="S19"/>
@@ -1874,52 +1874,52 @@
         <v>43</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.0398196785230777</v>
+        <v>-0.0402713131564558</v>
       </c>
       <c r="C20" t="n">
-        <v>0.01644831839626</v>
+        <v>0.0160716467382088</v>
       </c>
       <c r="D20" t="n">
-        <v>-2.4208966268632</v>
+        <v>-2.50573658147392</v>
       </c>
       <c r="E20" t="n">
-        <v>0.0356826532899045</v>
+        <v>0.0307862534522951</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.0541166078435905</v>
+        <v>-0.0532385085864461</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0185288272727632</v>
+        <v>0.0184205487209443</v>
       </c>
       <c r="H20" t="n">
-        <v>-2.9206709656763</v>
+        <v>-2.89016952713866</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0150394493225655</v>
+        <v>0.0158097223100596</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.0272385728801503</v>
+        <v>-0.0270596788537417</v>
       </c>
       <c r="K20" t="n">
-        <v>0.0374106238604845</v>
+        <v>0.0372511962563195</v>
       </c>
       <c r="L20" t="n">
-        <v>-0.728097264074802</v>
+        <v>-0.726411003489617</v>
       </c>
       <c r="M20" t="n">
-        <v>0.483068396733963</v>
+        <v>0.484010977240596</v>
       </c>
       <c r="N20" t="n">
-        <v>-0.00186820114666191</v>
+        <v>-0.00115674982091235</v>
       </c>
       <c r="O20" t="n">
-        <v>0.0407004496156528</v>
+        <v>0.0405929540994348</v>
       </c>
       <c r="P20" t="n">
-        <v>-0.0459012410011173</v>
+        <v>-0.0284963202746669</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.964283952652152</v>
+        <v>0.977820029380574</v>
       </c>
       <c r="R20"/>
       <c r="S20"/>
@@ -1935,52 +1935,52 @@
         <v>44</v>
       </c>
       <c r="B21" t="n">
-        <v>0.111002501859107</v>
+        <v>0.109380736493537</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0119834648311757</v>
+        <v>0.0109176246057166</v>
       </c>
       <c r="D21" t="n">
-        <v>9.26297222238497</v>
+        <v>10.018730304783</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0000000899873576765739</v>
+        <v>0.0000000310258154273521</v>
       </c>
       <c r="F21" t="n">
-        <v>0.120306975367787</v>
+        <v>0.119434487919124</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0149882086477381</v>
+        <v>0.0149422765822124</v>
       </c>
       <c r="H21" t="n">
-        <v>8.02677479312664</v>
+        <v>7.99305830420116</v>
       </c>
       <c r="I21" t="n">
-        <v>0.000000596021191846155</v>
+        <v>0.000000629478894873684</v>
       </c>
       <c r="J21" t="n">
-        <v>0.152094807689525</v>
+        <v>0.150882597326848</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0188343035933845</v>
+        <v>0.0187937879672495</v>
       </c>
       <c r="L21" t="n">
-        <v>8.07541446570649</v>
+        <v>8.02832284741001</v>
       </c>
       <c r="M21" t="n">
-        <v>0.000000535531671344761</v>
+        <v>0.000000577916155050134</v>
       </c>
       <c r="N21" t="n">
-        <v>0.151262942495892</v>
+        <v>0.149904732839406</v>
       </c>
       <c r="O21" t="n">
-        <v>0.0252749043282427</v>
+        <v>0.0257562426751398</v>
       </c>
       <c r="P21" t="n">
-        <v>5.98470880567756</v>
+        <v>5.82013202508359</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.0000197427969935556</v>
+        <v>0.0000269755355429609</v>
       </c>
       <c r="R21"/>
       <c r="S21"/>
@@ -1996,52 +1996,52 @@
         <v>45</v>
       </c>
       <c r="B22" t="n">
-        <v>0.0541135821292939</v>
+        <v>0.0551902130678575</v>
       </c>
       <c r="C22" t="n">
-        <v>0.00482809151981211</v>
+        <v>0.0047198074239534</v>
       </c>
       <c r="D22" t="n">
-        <v>11.208068841951</v>
+        <v>11.6933188391888</v>
       </c>
       <c r="E22" t="n">
-        <v>0.00000000441511267512479</v>
+        <v>0.00000000238210644915438</v>
       </c>
       <c r="F22" t="n">
-        <v>0.0577724733232997</v>
+        <v>0.0584639434559015</v>
       </c>
       <c r="G22" t="n">
-        <v>0.00657263938149583</v>
+        <v>0.00636148229701379</v>
       </c>
       <c r="H22" t="n">
-        <v>8.78984377051758</v>
+        <v>9.19030199665032</v>
       </c>
       <c r="I22" t="n">
-        <v>0.000000136467058642478</v>
+        <v>0.0000000740664371070864</v>
       </c>
       <c r="J22" t="n">
-        <v>0.0708682622427438</v>
+        <v>0.0716436235914391</v>
       </c>
       <c r="K22" t="n">
-        <v>0.0116575386854812</v>
+        <v>0.0114794570293101</v>
       </c>
       <c r="L22" t="n">
-        <v>6.07917881765267</v>
+        <v>6.24102894488077</v>
       </c>
       <c r="M22" t="n">
-        <v>0.0000146025443874357</v>
+        <v>0.0000107472547688733</v>
       </c>
       <c r="N22" t="n">
-        <v>0.0675865244161758</v>
+        <v>0.0690856575897439</v>
       </c>
       <c r="O22" t="n">
-        <v>0.0137556430775895</v>
+        <v>0.0131297978427418</v>
       </c>
       <c r="P22" t="n">
-        <v>4.91336712031201</v>
+        <v>5.26174571895139</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.000145677706268544</v>
+        <v>0.0000717026243251659</v>
       </c>
       <c r="R22"/>
       <c r="S22"/>
@@ -2057,52 +2057,52 @@
         <v>46</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.0561103427779548</v>
+        <v>-0.0575077118462967</v>
       </c>
       <c r="C23" t="n">
-        <v>0.00948867771165978</v>
+        <v>0.00945622613825679</v>
       </c>
       <c r="D23" t="n">
-        <v>-5.91339957821582</v>
+        <v>-6.08146537587964</v>
       </c>
       <c r="E23" t="n">
-        <v>0.0000130188981584221</v>
+        <v>0.00000920454639596171</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.0586141384645751</v>
+        <v>-0.058652746448475</v>
       </c>
       <c r="G23" t="n">
-        <v>0.00920373332094904</v>
+        <v>0.00922116937747314</v>
       </c>
       <c r="H23" t="n">
-        <v>-6.36851768957286</v>
+        <v>-6.36066251984924</v>
       </c>
       <c r="I23" t="n">
-        <v>0.00000514694933560008</v>
+        <v>0.00000522724367591758</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.0572899106601977</v>
+        <v>-0.0574485255082733</v>
       </c>
       <c r="K23" t="n">
-        <v>0.015023776857067</v>
+        <v>0.0151015057616902</v>
       </c>
       <c r="L23" t="n">
-        <v>-3.81328285192478</v>
+        <v>-3.80415876501599</v>
       </c>
       <c r="M23" t="n">
-        <v>0.00125802989312195</v>
+        <v>0.00128384963320015</v>
       </c>
       <c r="N23" t="n">
-        <v>-0.0290865166550079</v>
+        <v>-0.0297279476469506</v>
       </c>
       <c r="O23" t="n">
-        <v>0.0163221047725256</v>
+        <v>0.0163870784485174</v>
       </c>
       <c r="P23" t="n">
-        <v>-1.78203222319514</v>
+        <v>-1.81410907016438</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.0914737431553872</v>
+        <v>0.0862183347396163</v>
       </c>
       <c r="R23"/>
       <c r="S23"/>
@@ -2118,40 +2118,40 @@
         <v>47</v>
       </c>
       <c r="B24" t="n">
-        <v>0.0178445116421963</v>
+        <v>0.0200243465278871</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0122654233054867</v>
+        <v>0.0118838168228605</v>
       </c>
       <c r="D24" t="n">
-        <v>1.45486308933291</v>
+        <v>1.68500969228733</v>
       </c>
       <c r="E24" t="n">
-        <v>0.167703667516122</v>
+        <v>0.114102353620347</v>
       </c>
       <c r="F24" t="n">
-        <v>0.0175938410980195</v>
+        <v>0.0182841150321371</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0129577464412309</v>
+        <v>0.0129986640210445</v>
       </c>
       <c r="H24" t="n">
-        <v>1.35778556694371</v>
+        <v>1.40661494154596</v>
       </c>
       <c r="I24" t="n">
-        <v>0.19596061166853</v>
+        <v>0.181327973479757</v>
       </c>
       <c r="J24" t="n">
-        <v>0.0403210483719435</v>
+        <v>0.0410002737608848</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0198381840344496</v>
+        <v>0.0198401524380298</v>
       </c>
       <c r="L24" t="n">
-        <v>2.03249694134931</v>
+        <v>2.06653017858346</v>
       </c>
       <c r="M24" t="n">
-        <v>0.0614626575953681</v>
+        <v>0.0577635329473402</v>
       </c>
       <c r="N24"/>
       <c r="O24"/>
@@ -2171,40 +2171,40 @@
         <v>48</v>
       </c>
       <c r="B25" t="n">
-        <v>-0.0308965948633378</v>
+        <v>-0.0380234358114318</v>
       </c>
       <c r="C25" t="n">
-        <v>0.03190818724459</v>
+        <v>0.026068493502605</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.968296776827279</v>
+        <v>-1.45859736035886</v>
       </c>
       <c r="E25" t="n">
-        <v>0.370032146311416</v>
+        <v>0.194597747165527</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.0351132953931947</v>
+        <v>-0.0355246954353174</v>
       </c>
       <c r="G25" t="n">
-        <v>0.0301547878339958</v>
+        <v>0.0303023475700999</v>
       </c>
       <c r="H25" t="n">
-        <v>-1.16443516653129</v>
+        <v>-1.17234136243525</v>
       </c>
       <c r="I25" t="n">
-        <v>0.288129760501284</v>
+        <v>0.28517562890227</v>
       </c>
       <c r="J25" t="n">
-        <v>-0.0285384446443436</v>
+        <v>-0.0294191079887068</v>
       </c>
       <c r="K25" t="n">
-        <v>0.0349764077459206</v>
+        <v>0.0349868646093803</v>
       </c>
       <c r="L25" t="n">
-        <v>-0.815934124843686</v>
+        <v>-0.840861515233329</v>
       </c>
       <c r="M25" t="n">
-        <v>0.445473559682882</v>
+        <v>0.432404667461159</v>
       </c>
       <c r="N25"/>
       <c r="O25"/>
@@ -2224,40 +2224,40 @@
         <v>49</v>
       </c>
       <c r="B26" t="n">
-        <v>-0.108319524210041</v>
+        <v>-0.10201934560745</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0270270211228442</v>
+        <v>0.0287475271523367</v>
       </c>
       <c r="D26" t="n">
-        <v>-4.00782327129961</v>
+        <v>-3.54880421772756</v>
       </c>
       <c r="E26" t="n">
-        <v>0.00162460035186023</v>
+        <v>0.00380257400060897</v>
       </c>
       <c r="F26" t="n">
-        <v>-0.0980416061341567</v>
+        <v>-0.0980067444068867</v>
       </c>
       <c r="G26" t="n">
-        <v>0.0260609475590279</v>
+        <v>0.0263016591721741</v>
       </c>
       <c r="H26" t="n">
-        <v>-3.76201233328501</v>
+        <v>-3.7262571066457</v>
       </c>
       <c r="I26" t="n">
-        <v>0.00256099343216476</v>
+        <v>0.00275204581218953</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.0695452506105122</v>
+        <v>-0.0701270569569188</v>
       </c>
       <c r="K26" t="n">
-        <v>0.0330526572579732</v>
+        <v>0.0329576974946572</v>
       </c>
       <c r="L26" t="n">
-        <v>-2.10407441881957</v>
+        <v>-2.12778993339226</v>
       </c>
       <c r="M26" t="n">
-        <v>0.0563411671771082</v>
+        <v>0.0540634108677966</v>
       </c>
       <c r="N26"/>
       <c r="O26"/>
@@ -2277,40 +2277,40 @@
         <v>50</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.0445612660740493</v>
+        <v>-0.0438695248599271</v>
       </c>
       <c r="C27" t="n">
-        <v>0.0599007856590607</v>
+        <v>0.0603283014528479</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.743917889953567</v>
+        <v>-0.727179844342463</v>
       </c>
       <c r="E27" t="n">
-        <v>0.474646738070378</v>
+        <v>0.484397684269179</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.018470611965199</v>
+        <v>-0.0161295604440727</v>
       </c>
       <c r="G27" t="n">
-        <v>0.0623403000197632</v>
+        <v>0.0622309510499517</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.296286863543221</v>
+        <v>-0.259188718345727</v>
       </c>
       <c r="I27" t="n">
-        <v>0.773247605151953</v>
+        <v>0.800902448340753</v>
       </c>
       <c r="J27" t="n">
-        <v>0.00867506234276572</v>
+        <v>0.0108455647645459</v>
       </c>
       <c r="K27" t="n">
-        <v>0.0702381325339788</v>
+        <v>0.0702351012864114</v>
       </c>
       <c r="L27" t="n">
-        <v>0.123509296585712</v>
+        <v>0.154418012730114</v>
       </c>
       <c r="M27" t="n">
-        <v>0.904173842480825</v>
+        <v>0.880382473395245</v>
       </c>
       <c r="N27"/>
       <c r="O27"/>
@@ -2330,40 +2330,40 @@
         <v>51</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.00806410862148786</v>
+        <v>-0.00783284807322008</v>
       </c>
       <c r="C28" t="n">
-        <v>0.0258973983074377</v>
+        <v>0.0270464980914847</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.31138682448931</v>
+        <v>-0.289606737505369</v>
       </c>
       <c r="E28" t="n">
-        <v>0.760859948482451</v>
+        <v>0.777241490934386</v>
       </c>
       <c r="F28" t="n">
-        <v>0.0129918227195937</v>
+        <v>0.0128012395992633</v>
       </c>
       <c r="G28" t="n">
-        <v>0.02361548004881</v>
+        <v>0.023726114161638</v>
       </c>
       <c r="H28" t="n">
-        <v>0.550140106944318</v>
+        <v>0.539542190181366</v>
       </c>
       <c r="I28" t="n">
-        <v>0.592327007573548</v>
+        <v>0.599752420404195</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.00829320566203946</v>
+        <v>-0.011653089722219</v>
       </c>
       <c r="K28" t="n">
-        <v>0.0236651196653828</v>
+        <v>0.0228328253280048</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.350440047601817</v>
+        <v>-0.510365649227225</v>
       </c>
       <c r="M28" t="n">
-        <v>0.732028895201571</v>
+        <v>0.619303762977731</v>
       </c>
       <c r="N28"/>
       <c r="O28"/>
@@ -2383,40 +2383,40 @@
         <v>52</v>
       </c>
       <c r="B29" t="n">
-        <v>-0.116248092671436</v>
+        <v>-0.120970662096327</v>
       </c>
       <c r="C29" t="n">
-        <v>0.173221153995579</v>
+        <v>0.18219468176145</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.671096398967547</v>
+        <v>-0.663963738824799</v>
       </c>
       <c r="E29" t="n">
-        <v>0.586798839225548</v>
+        <v>0.590811924329395</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.09195000421162</v>
+        <v>-0.0874840635900641</v>
       </c>
       <c r="G29" t="n">
-        <v>0.191219910590606</v>
+        <v>0.191190863055805</v>
       </c>
       <c r="H29" t="n">
-        <v>-0.480859989567096</v>
+        <v>-0.457574500118917</v>
       </c>
       <c r="I29" t="n">
-        <v>0.6893121197212</v>
+        <v>0.702770621147571</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.0836384222368732</v>
+        <v>-0.0783099882690411</v>
       </c>
       <c r="K29" t="n">
-        <v>0.197216532028084</v>
+        <v>0.197490356876145</v>
       </c>
       <c r="L29" t="n">
-        <v>-0.424094376758247</v>
+        <v>-0.39652563045472</v>
       </c>
       <c r="M29" t="n">
-        <v>0.722636077306344</v>
+        <v>0.739191624398994</v>
       </c>
       <c r="N29"/>
       <c r="O29"/>
@@ -2436,40 +2436,40 @@
         <v>53</v>
       </c>
       <c r="B30" t="n">
-        <v>0.0322028723727278</v>
+        <v>0.0281698751124642</v>
       </c>
       <c r="C30" t="n">
-        <v>0.031078651744882</v>
+        <v>0.0301517453421998</v>
       </c>
       <c r="D30" t="n">
-        <v>1.03617340408053</v>
+        <v>0.934270132383952</v>
       </c>
       <c r="E30" t="n">
-        <v>0.316785244132208</v>
+        <v>0.365211146995218</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0141963345440114</v>
+        <v>0.0159684065197297</v>
       </c>
       <c r="G30" t="n">
-        <v>0.0340255443620326</v>
+        <v>0.0332787678752994</v>
       </c>
       <c r="H30" t="n">
-        <v>0.417225787571892</v>
+        <v>0.479837672463288</v>
       </c>
       <c r="I30" t="n">
-        <v>0.682511745334586</v>
+        <v>0.638377670002839</v>
       </c>
       <c r="J30" t="n">
-        <v>-0.0168346416620239</v>
+        <v>-0.0163635790921715</v>
       </c>
       <c r="K30" t="n">
-        <v>0.0396819547761611</v>
+        <v>0.0396582818650644</v>
       </c>
       <c r="L30" t="n">
-        <v>-0.424239223016738</v>
+        <v>-0.412614423081865</v>
       </c>
       <c r="M30" t="n">
-        <v>0.677507926050346</v>
+        <v>0.685826325518918</v>
       </c>
       <c r="N30"/>
       <c r="O30"/>
@@ -2489,40 +2489,40 @@
         <v>54</v>
       </c>
       <c r="B31" t="n">
-        <v>-0.0450676269900745</v>
+        <v>-0.0490517123499113</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0221006528404033</v>
+        <v>0.0234430463078594</v>
       </c>
       <c r="D31" t="n">
-        <v>-2.03919890129599</v>
+        <v>-2.09237791478774</v>
       </c>
       <c r="E31" t="n">
-        <v>0.0635133805249011</v>
+        <v>0.0577806615525232</v>
       </c>
       <c r="F31" t="n">
-        <v>-0.0519738546654739</v>
+        <v>-0.0543289166398147</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0235831708553669</v>
+        <v>0.0228990362311558</v>
       </c>
       <c r="H31" t="n">
-        <v>-2.20385354387771</v>
+        <v>-2.37254162539366</v>
       </c>
       <c r="I31" t="n">
-        <v>0.0472780508145726</v>
+        <v>0.0347783664103067</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.090788176913481</v>
+        <v>-0.0934833906177806</v>
       </c>
       <c r="K31" t="n">
-        <v>0.0356358558585655</v>
+        <v>0.0352751660649107</v>
       </c>
       <c r="L31" t="n">
-        <v>-2.54766371470938</v>
+        <v>-2.65011907940446</v>
       </c>
       <c r="M31" t="n">
-        <v>0.0251524670684022</v>
+        <v>0.0207967401207911</v>
       </c>
       <c r="N31"/>
       <c r="O31"/>
@@ -2542,40 +2542,40 @@
         <v>55</v>
       </c>
       <c r="B32" t="n">
-        <v>0.199085782693569</v>
+        <v>0.193414392289039</v>
       </c>
       <c r="C32" t="n">
-        <v>0.0406759643256926</v>
+        <v>0.0403069046618299</v>
       </c>
       <c r="D32" t="n">
-        <v>4.89443301453133</v>
+        <v>4.79854243117309</v>
       </c>
       <c r="E32" t="n">
-        <v>0.000310166754097686</v>
+        <v>0.000379584380109137</v>
       </c>
       <c r="F32" t="n">
-        <v>0.207064325449936</v>
+        <v>0.208456803793652</v>
       </c>
       <c r="G32" t="n">
-        <v>0.0417072451300645</v>
+        <v>0.0410072298851376</v>
       </c>
       <c r="H32" t="n">
-        <v>4.96470876472909</v>
+        <v>5.08341588489506</v>
       </c>
       <c r="I32" t="n">
-        <v>0.000274322880160753</v>
+        <v>0.000232608613348052</v>
       </c>
       <c r="J32" t="n">
-        <v>0.178635489217578</v>
+        <v>0.178052445244413</v>
       </c>
       <c r="K32" t="n">
-        <v>0.0470555830245081</v>
+        <v>0.0470252022910634</v>
       </c>
       <c r="L32" t="n">
-        <v>3.79626555948821</v>
+        <v>3.78631960246241</v>
       </c>
       <c r="M32" t="n">
-        <v>0.00232278544254728</v>
+        <v>0.00242294158585706</v>
       </c>
       <c r="N32"/>
       <c r="O32"/>
@@ -2595,40 +2595,40 @@
         <v>56</v>
       </c>
       <c r="B33" t="n">
-        <v>0.0111476351331794</v>
+        <v>-0.010905637813304</v>
       </c>
       <c r="C33" t="n">
-        <v>0.0900553406918359</v>
+        <v>0.104673463511094</v>
       </c>
       <c r="D33" t="n">
-        <v>0.123786496697913</v>
+        <v>-0.104187226136338</v>
       </c>
       <c r="E33" t="n">
-        <v>0.911724839796021</v>
+        <v>0.925607374815006</v>
       </c>
       <c r="F33" t="n">
-        <v>-0.0353044227098172</v>
+        <v>-0.0340194584568917</v>
       </c>
       <c r="G33" t="n">
-        <v>0.108454208873033</v>
+        <v>0.108451253089901</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.32552376783411</v>
+        <v>-0.313684328098001</v>
       </c>
       <c r="I33" t="n">
-        <v>0.77296725360542</v>
+        <v>0.780840372839301</v>
       </c>
       <c r="J33" t="n">
-        <v>-0.0100005236829128</v>
+        <v>-0.0111477450037464</v>
       </c>
       <c r="K33" t="n">
-        <v>0.044023363260131</v>
+        <v>0.0445414969826509</v>
       </c>
       <c r="L33" t="n">
-        <v>-0.227164008888198</v>
+        <v>-0.250277735570687</v>
       </c>
       <c r="M33" t="n">
-        <v>0.842670800181233</v>
+        <v>0.827132918440743</v>
       </c>
       <c r="N33"/>
       <c r="O33"/>
@@ -2648,40 +2648,40 @@
         <v>57</v>
       </c>
       <c r="B34" t="n">
-        <v>-0.0260025403048048</v>
+        <v>-0.0104505573719072</v>
       </c>
       <c r="C34" t="n">
-        <v>0.0586039338818581</v>
+        <v>0.0590071628862223</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.44369957070159</v>
+        <v>-0.177106589450132</v>
       </c>
       <c r="E34" t="n">
-        <v>0.669066684807665</v>
+        <v>0.863860079964858</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.046348946633261</v>
+        <v>-0.0452030191051732</v>
       </c>
       <c r="G34" t="n">
-        <v>0.0551917989653559</v>
+        <v>0.0554798219031849</v>
       </c>
       <c r="H34" t="n">
-        <v>-0.839779595920661</v>
+        <v>-0.814765036269489</v>
       </c>
       <c r="I34" t="n">
-        <v>0.426085142571577</v>
+        <v>0.439397407084801</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.000304865919649459</v>
+        <v>0.00141139312021738</v>
       </c>
       <c r="K34" t="n">
-        <v>0.0627736746380938</v>
+        <v>0.0634870490551861</v>
       </c>
       <c r="L34" t="n">
-        <v>-0.00485658871186192</v>
+        <v>0.0222311974051672</v>
       </c>
       <c r="M34" t="n">
-        <v>0.996250130850443</v>
+        <v>0.982835297839643</v>
       </c>
       <c r="N34"/>
       <c r="O34"/>
@@ -2701,40 +2701,40 @@
         <v>58</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.0591737804177147</v>
+        <v>-0.0672437082872521</v>
       </c>
       <c r="C35" t="n">
-        <v>0.0376835947004212</v>
+        <v>0.0320070933581677</v>
       </c>
       <c r="D35" t="n">
-        <v>-1.57027961074672</v>
+        <v>-2.10090018280565</v>
       </c>
       <c r="E35" t="n">
-        <v>0.168850948343375</v>
+        <v>0.081628838197055</v>
       </c>
       <c r="F35" t="n">
-        <v>-0.038408778057036</v>
+        <v>-0.0383826727597701</v>
       </c>
       <c r="G35" t="n">
-        <v>0.0380460807350373</v>
+        <v>0.0379240028121578</v>
       </c>
       <c r="H35" t="n">
-        <v>-1.00953310603856</v>
+        <v>-1.0120944497838</v>
       </c>
       <c r="I35" t="n">
-        <v>0.352570087029119</v>
+        <v>0.351623723416501</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.0629007748738643</v>
+        <v>-0.0619944217553618</v>
       </c>
       <c r="K35" t="n">
-        <v>0.0518568350069654</v>
+        <v>0.0517307561306496</v>
       </c>
       <c r="L35" t="n">
-        <v>-1.21296980167447</v>
+        <v>-1.19840548239408</v>
       </c>
       <c r="M35" t="n">
-        <v>0.272597854944578</v>
+        <v>0.277989681589115</v>
       </c>
       <c r="N35"/>
       <c r="O35"/>
@@ -2754,40 +2754,40 @@
         <v>59</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.0780048399459508</v>
+        <v>-0.0761410983629715</v>
       </c>
       <c r="C36" t="n">
-        <v>0.0543918013935141</v>
+        <v>0.0532715920813476</v>
       </c>
       <c r="D36" t="n">
-        <v>-1.43412863607147</v>
+        <v>-1.4293002215271</v>
       </c>
       <c r="E36" t="n">
-        <v>0.172484906772889</v>
+        <v>0.173942658703668</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.0954092920867933</v>
+        <v>-0.0944133184235534</v>
       </c>
       <c r="G36" t="n">
-        <v>0.0508571471123413</v>
+        <v>0.0502922930389514</v>
       </c>
       <c r="H36" t="n">
-        <v>-1.87602524923465</v>
+        <v>-1.87729198090909</v>
       </c>
       <c r="I36" t="n">
-        <v>0.0803262227026076</v>
+        <v>0.0801326633969434</v>
       </c>
       <c r="J36" t="n">
-        <v>-0.0744281267890858</v>
+        <v>-0.0730908723237833</v>
       </c>
       <c r="K36" t="n">
-        <v>0.0520229662144112</v>
+        <v>0.0513027547344179</v>
       </c>
       <c r="L36" t="n">
-        <v>-1.43067826010406</v>
+        <v>-1.42469683552389</v>
       </c>
       <c r="M36" t="n">
-        <v>0.17472076816231</v>
+        <v>0.17638610194021</v>
       </c>
       <c r="N36"/>
       <c r="O36"/>
@@ -2807,40 +2807,40 @@
         <v>60</v>
       </c>
       <c r="B37" t="n">
-        <v>0.05192364394294</v>
+        <v>0.0454962291916527</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0587372789599473</v>
+        <v>0.0585902800670022</v>
       </c>
       <c r="D37" t="n">
-        <v>0.883998116057547</v>
+        <v>0.776514963567753</v>
       </c>
       <c r="E37" t="n">
-        <v>0.4045404901179</v>
+        <v>0.461848973941789</v>
       </c>
       <c r="F37" t="n">
-        <v>0.00880479772945048</v>
+        <v>0.0136435357635563</v>
       </c>
       <c r="G37" t="n">
-        <v>0.0780946768716221</v>
+        <v>0.0791759041462967</v>
       </c>
       <c r="H37" t="n">
-        <v>0.112745171401688</v>
+        <v>0.172319292222373</v>
       </c>
       <c r="I37" t="n">
-        <v>0.913312822451942</v>
+        <v>0.867907625401763</v>
       </c>
       <c r="J37" t="n">
-        <v>0.0952730154001841</v>
+        <v>0.101149532272405</v>
       </c>
       <c r="K37" t="n">
-        <v>0.0795455676798426</v>
+        <v>0.0813819412754367</v>
       </c>
       <c r="L37" t="n">
-        <v>1.19771620442313</v>
+        <v>1.24289898578439</v>
       </c>
       <c r="M37" t="n">
-        <v>0.270937580577534</v>
+        <v>0.25467441044358</v>
       </c>
       <c r="N37"/>
       <c r="O37"/>
@@ -2860,40 +2860,40 @@
         <v>61</v>
       </c>
       <c r="B38" t="n">
-        <v>0.0171523376220814</v>
+        <v>-0.00754839967530409</v>
       </c>
       <c r="C38" t="n">
-        <v>0.145754258498652</v>
+        <v>0.143803883483802</v>
       </c>
       <c r="D38" t="n">
-        <v>0.117679838645949</v>
+        <v>-0.052490930651079</v>
       </c>
       <c r="E38" t="n">
-        <v>0.908278824141981</v>
+        <v>0.959006324127802</v>
       </c>
       <c r="F38" t="n">
-        <v>0.0776094309319206</v>
+        <v>0.0717717531577842</v>
       </c>
       <c r="G38" t="n">
-        <v>0.14055767100751</v>
+        <v>0.135873953022679</v>
       </c>
       <c r="H38" t="n">
-        <v>0.552153648930153</v>
+        <v>0.528223044675862</v>
       </c>
       <c r="I38" t="n">
-        <v>0.591444253236501</v>
+        <v>0.607474231057697</v>
       </c>
       <c r="J38" t="n">
-        <v>0.169621862756514</v>
+        <v>0.161912786573172</v>
       </c>
       <c r="K38" t="n">
-        <v>0.152001263966858</v>
+        <v>0.146219345439956</v>
       </c>
       <c r="L38" t="n">
-        <v>1.11592402806268</v>
+        <v>1.10732807677394</v>
       </c>
       <c r="M38" t="n">
-        <v>0.288190122225791</v>
+        <v>0.291900769578197</v>
       </c>
       <c r="N38"/>
       <c r="O38"/>
@@ -2913,40 +2913,40 @@
         <v>62</v>
       </c>
       <c r="B39" t="n">
-        <v>0.26039517131502</v>
+        <v>0.268882161840341</v>
       </c>
       <c r="C39" t="n">
-        <v>0.124689969701545</v>
+        <v>0.138273316745694</v>
       </c>
       <c r="D39" t="n">
-        <v>2.08834096229469</v>
+        <v>1.94457013231885</v>
       </c>
       <c r="E39" t="n">
-        <v>0.136464364173298</v>
+        <v>0.15440710803952</v>
       </c>
       <c r="F39" t="n">
-        <v>0.557072680642449</v>
+        <v>0.559811041837543</v>
       </c>
       <c r="G39" t="n">
-        <v>0.185098931678213</v>
+        <v>0.188239854159493</v>
       </c>
       <c r="H39" t="n">
-        <v>3.00959425098626</v>
+        <v>2.97392411578911</v>
       </c>
       <c r="I39" t="n">
-        <v>0.0706876580539969</v>
+        <v>0.0724393178717576</v>
       </c>
       <c r="J39" t="n">
-        <v>0.633741664742215</v>
+        <v>0.637371713431108</v>
       </c>
       <c r="K39" t="n">
-        <v>0.1292926378557</v>
+        <v>0.133058104567209</v>
       </c>
       <c r="L39" t="n">
-        <v>4.9016067368779</v>
+        <v>4.79017580706002</v>
       </c>
       <c r="M39" t="n">
-        <v>0.0249866931099103</v>
+        <v>0.0263212536701611</v>
       </c>
       <c r="N39"/>
       <c r="O39"/>
@@ -2966,40 +2966,40 @@
         <v>63</v>
       </c>
       <c r="B40" t="n">
-        <v>0.395493544674451</v>
+        <v>0.406542278021684</v>
       </c>
       <c r="C40" t="n">
-        <v>0.0345514597315122</v>
+        <v>0.033659306053554</v>
       </c>
       <c r="D40" t="n">
-        <v>11.4465075498314</v>
+        <v>12.0781538803815</v>
       </c>
       <c r="E40" t="n">
-        <v>0.00402967644228015</v>
+        <v>0.00345089064364275</v>
       </c>
       <c r="F40" t="n">
-        <v>0.350077064311879</v>
+        <v>0.34991244025478</v>
       </c>
       <c r="G40" t="n">
-        <v>0.0532071026495113</v>
+        <v>0.0540805659745229</v>
       </c>
       <c r="H40" t="n">
-        <v>6.57951752452911</v>
+        <v>6.47020669901314</v>
       </c>
       <c r="I40" t="n">
-        <v>0.0160842658479906</v>
+        <v>0.0166806084879946</v>
       </c>
       <c r="J40" t="n">
-        <v>0.354842793170012</v>
+        <v>0.35370164192287</v>
       </c>
       <c r="K40" t="n">
-        <v>0.0617590895341362</v>
+        <v>0.0623898782979658</v>
       </c>
       <c r="L40" t="n">
-        <v>5.74559624901658</v>
+        <v>5.66921512867261</v>
       </c>
       <c r="M40" t="n">
-        <v>0.0215322408920702</v>
+        <v>0.0221576142119755</v>
       </c>
       <c r="N40"/>
       <c r="O40"/>
@@ -3019,40 +3019,40 @@
         <v>64</v>
       </c>
       <c r="B41" t="n">
-        <v>0.615300597475659</v>
+        <v>0.621700906782957</v>
       </c>
       <c r="C41" t="n">
-        <v>0.0506179413481717</v>
+        <v>0.0507914104428809</v>
       </c>
       <c r="D41" t="n">
-        <v>12.1557807585133</v>
+        <v>12.240276483011</v>
       </c>
       <c r="E41" t="n">
-        <v>0.000556280892032859</v>
+        <v>0.000510599399355029</v>
       </c>
       <c r="F41" t="n">
-        <v>0.574876172244976</v>
+        <v>0.573408903401983</v>
       </c>
       <c r="G41" t="n">
-        <v>0.0744136026823301</v>
+        <v>0.0743119708798414</v>
       </c>
       <c r="H41" t="n">
-        <v>7.72541782043679</v>
+        <v>7.71623867074062</v>
       </c>
       <c r="I41" t="n">
-        <v>0.00310156761522408</v>
+        <v>0.00305398970147893</v>
       </c>
       <c r="J41" t="n">
-        <v>0.597181490267554</v>
+        <v>0.595886816455256</v>
       </c>
       <c r="K41" t="n">
-        <v>0.086010537139314</v>
+        <v>0.0867528923807017</v>
       </c>
       <c r="L41" t="n">
-        <v>6.94312011213557</v>
+        <v>6.86878327745314</v>
       </c>
       <c r="M41" t="n">
-        <v>0.00447915401449055</v>
+        <v>0.00455723132421699</v>
       </c>
       <c r="N41"/>
       <c r="O41"/>
@@ -3072,40 +3072,40 @@
         <v>65</v>
       </c>
       <c r="B42" t="n">
-        <v>0.612556222628202</v>
+        <v>0.624552447373061</v>
       </c>
       <c r="C42" t="n">
-        <v>0.0566991109323759</v>
+        <v>0.0611337642201625</v>
       </c>
       <c r="D42" t="n">
-        <v>10.8036301196819</v>
+        <v>10.2161621378956</v>
       </c>
       <c r="E42" t="n">
-        <v>0.0000287539755911905</v>
+        <v>0.0000387806069031006</v>
       </c>
       <c r="F42" t="n">
-        <v>0.569348091186197</v>
+        <v>0.570055896590108</v>
       </c>
       <c r="G42" t="n">
-        <v>0.086384520983523</v>
+        <v>0.0878479894478355</v>
       </c>
       <c r="H42" t="n">
-        <v>6.59085776831238</v>
+        <v>6.48911716902309</v>
       </c>
       <c r="I42" t="n">
-        <v>0.000566489011109645</v>
+        <v>0.000610098308121154</v>
       </c>
       <c r="J42" t="n">
-        <v>0.582689930101248</v>
+        <v>0.58341196665216</v>
       </c>
       <c r="K42" t="n">
-        <v>0.0973199510563033</v>
+        <v>0.0993793605324924</v>
       </c>
       <c r="L42" t="n">
-        <v>5.9873635752667</v>
+        <v>5.87055464561388</v>
       </c>
       <c r="M42" t="n">
-        <v>0.00095450534855674</v>
+        <v>0.0010506303178264</v>
       </c>
       <c r="N42"/>
       <c r="O42"/>
@@ -3125,40 +3125,40 @@
         <v>66</v>
       </c>
       <c r="B43" t="n">
-        <v>0.628790027651101</v>
+        <v>0.637767854631027</v>
       </c>
       <c r="C43" t="n">
-        <v>0.045532079460468</v>
+        <v>0.0487074526955753</v>
       </c>
       <c r="D43" t="n">
-        <v>13.8098245259593</v>
+        <v>13.0938453837263</v>
       </c>
       <c r="E43" t="n">
-        <v>0.0000227054023141478</v>
+        <v>0.0000290442678371008</v>
       </c>
       <c r="F43" t="n">
-        <v>0.589492381479519</v>
+        <v>0.589003600817558</v>
       </c>
       <c r="G43" t="n">
-        <v>0.0752643365298626</v>
+        <v>0.0759383863206158</v>
       </c>
       <c r="H43" t="n">
-        <v>7.83229360223785</v>
+        <v>7.75633548928409</v>
       </c>
       <c r="I43" t="n">
-        <v>0.000490783986540143</v>
+        <v>0.000508085163026597</v>
       </c>
       <c r="J43" t="n">
-        <v>0.599300783382746</v>
+        <v>0.598547325153545</v>
       </c>
       <c r="K43" t="n">
-        <v>0.0882993091595741</v>
+        <v>0.0893805050425915</v>
       </c>
       <c r="L43" t="n">
-        <v>6.78715144078526</v>
+        <v>6.69662053115863</v>
       </c>
       <c r="M43" t="n">
-        <v>0.00100086998324887</v>
+        <v>0.00105499701313815</v>
       </c>
       <c r="N43"/>
       <c r="O43"/>
@@ -3178,40 +3178,40 @@
         <v>67</v>
       </c>
       <c r="B44" t="n">
-        <v>0.570093252589247</v>
+        <v>0.582196694695761</v>
       </c>
       <c r="C44" t="n">
-        <v>0.0402711600034478</v>
+        <v>0.0478862550087751</v>
       </c>
       <c r="D44" t="n">
-        <v>14.1563653130538</v>
+        <v>12.1579082471384</v>
       </c>
       <c r="E44" t="n">
-        <v>0.00000028700982770756</v>
+        <v>0.00000102113593260828</v>
       </c>
       <c r="F44" t="n">
-        <v>0.518707149490123</v>
+        <v>0.520095954911607</v>
       </c>
       <c r="G44" t="n">
-        <v>0.0809439083531574</v>
+        <v>0.0824256020707989</v>
       </c>
       <c r="H44" t="n">
-        <v>6.40822960051557</v>
+        <v>6.30988360224381</v>
       </c>
       <c r="I44" t="n">
-        <v>0.000166759086069445</v>
+        <v>0.000184708288760526</v>
       </c>
       <c r="J44" t="n">
-        <v>0.520625705170581</v>
+        <v>0.5219991141145</v>
       </c>
       <c r="K44" t="n">
-        <v>0.0952881277026678</v>
+        <v>0.097258015835895</v>
       </c>
       <c r="L44" t="n">
-        <v>5.46369959954629</v>
+        <v>5.36715775690178</v>
       </c>
       <c r="M44" t="n">
-        <v>0.000513793463402316</v>
+        <v>0.000575635767322483</v>
       </c>
       <c r="N44"/>
       <c r="O44"/>
@@ -3231,40 +3231,40 @@
         <v>68</v>
       </c>
       <c r="B45" t="n">
-        <v>0.00000298573357907324</v>
+        <v>-0.00000320257979612728</v>
       </c>
       <c r="C45" t="n">
-        <v>0.000133130473279937</v>
+        <v>0.000123499197277699</v>
       </c>
       <c r="D45" t="n">
-        <v>0.0224271235992308</v>
+        <v>-0.0259319887636678</v>
       </c>
       <c r="E45" t="n">
-        <v>0.982614918632978</v>
+        <v>0.979899170337162</v>
       </c>
       <c r="F45" t="n">
-        <v>0.000100315412591254</v>
+        <v>0.000114751921224352</v>
       </c>
       <c r="G45" t="n">
-        <v>0.000141446609642101</v>
+        <v>0.000135641091504213</v>
       </c>
       <c r="H45" t="n">
-        <v>0.709210442336368</v>
+        <v>0.845996740012873</v>
       </c>
       <c r="I45" t="n">
-        <v>0.497310264328012</v>
+        <v>0.420869742825734</v>
       </c>
       <c r="J45" t="n">
-        <v>-0.000162589106792985</v>
+        <v>-0.000144252246204352</v>
       </c>
       <c r="K45" t="n">
-        <v>0.000240846771734823</v>
+        <v>0.000234116954526647</v>
       </c>
       <c r="L45" t="n">
-        <v>-0.675072809246529</v>
+        <v>-0.616154633038048</v>
       </c>
       <c r="M45" t="n">
-        <v>0.518247508577196</v>
+        <v>0.554520341790022</v>
       </c>
       <c r="N45"/>
       <c r="O45"/>
@@ -3284,40 +3284,40 @@
         <v>69</v>
       </c>
       <c r="B46" t="n">
-        <v>0.00499112097633194</v>
+        <v>0.00517943882886705</v>
       </c>
       <c r="C46" t="n">
-        <v>0.00387706680263973</v>
+        <v>0.00412614901564003</v>
       </c>
       <c r="D46" t="n">
-        <v>1.28734459074414</v>
+        <v>1.25527187923523</v>
       </c>
       <c r="E46" t="n">
-        <v>0.216552615752047</v>
+        <v>0.22766087407428</v>
       </c>
       <c r="F46" t="n">
-        <v>-0.000731659886759521</v>
+        <v>0.0000269320739364195</v>
       </c>
       <c r="G46" t="n">
-        <v>0.00421391512668558</v>
+        <v>0.00406858406929453</v>
       </c>
       <c r="H46" t="n">
-        <v>-0.173629478706421</v>
+        <v>0.00661952007817043</v>
       </c>
       <c r="I46" t="n">
-        <v>0.864367555371537</v>
+        <v>0.994801509196308</v>
       </c>
       <c r="J46" t="n">
-        <v>-0.00972131629430284</v>
+        <v>-0.0088294720735663</v>
       </c>
       <c r="K46" t="n">
-        <v>0.00586261214042788</v>
+        <v>0.00581735707209573</v>
       </c>
       <c r="L46" t="n">
-        <v>-1.65818854487504</v>
+        <v>-1.517780662961</v>
       </c>
       <c r="M46" t="n">
-        <v>0.117014161625359</v>
+        <v>0.148842426562061</v>
       </c>
       <c r="N46"/>
       <c r="O46"/>
@@ -3337,40 +3337,40 @@
         <v>70</v>
       </c>
       <c r="B47" t="n">
-        <v>0.0104265654443451</v>
+        <v>0.00543798563862362</v>
       </c>
       <c r="C47" t="n">
-        <v>0.00414560478000441</v>
+        <v>0.00234785594508243</v>
       </c>
       <c r="D47" t="n">
-        <v>2.51508911187961</v>
+        <v>2.31614961301754</v>
       </c>
       <c r="E47" t="n">
-        <v>0.0810582020773294</v>
+        <v>0.0935788548229598</v>
       </c>
       <c r="F47" t="n">
-        <v>0.0155085568628634</v>
+        <v>0.0123473496881596</v>
       </c>
       <c r="G47" t="n">
-        <v>0.00357231379435102</v>
+        <v>0.00391156437859763</v>
       </c>
       <c r="H47" t="n">
-        <v>4.34131987155983</v>
+        <v>3.15662698937514</v>
       </c>
       <c r="I47" t="n">
-        <v>0.0201386103514258</v>
+        <v>0.0440110044294618</v>
       </c>
       <c r="J47" t="n">
-        <v>0.0211284102410065</v>
+        <v>0.0171954325559305</v>
       </c>
       <c r="K47" t="n">
-        <v>0.00243394572970819</v>
+        <v>0.00254602639572326</v>
       </c>
       <c r="L47" t="n">
-        <v>8.68072364273282</v>
+        <v>6.75383121903795</v>
       </c>
       <c r="M47" t="n">
-        <v>0.00256243809678317</v>
+        <v>0.0046174338071109</v>
       </c>
       <c r="N47"/>
       <c r="O47"/>
@@ -3390,28 +3390,28 @@
         <v>71</v>
       </c>
       <c r="B48" t="n">
-        <v>-0.00502406165581815</v>
+        <v>-0.00496105826458808</v>
       </c>
       <c r="C48" t="n">
-        <v>0.00743029792806135</v>
+        <v>0.00727586624528211</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.676158843758367</v>
+        <v>-0.681851218444948</v>
       </c>
       <c r="E48" t="n">
-        <v>0.515170493536377</v>
+        <v>0.511817625160581</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.00907464118658271</v>
+        <v>-0.00868740707985766</v>
       </c>
       <c r="G48" t="n">
-        <v>0.00971187541670845</v>
+        <v>0.00965461040612054</v>
       </c>
       <c r="H48" t="n">
-        <v>-0.934386078611611</v>
+        <v>-0.899819538481872</v>
       </c>
       <c r="I48" t="n">
-        <v>0.373070888263641</v>
+        <v>0.390302023126585</v>
       </c>
       <c r="J48"/>
       <c r="K48"/>
@@ -3435,28 +3435,28 @@
         <v>72</v>
       </c>
       <c r="B49" t="n">
-        <v>-0.0558544398741821</v>
+        <v>-0.0640134844320122</v>
       </c>
       <c r="C49" t="n">
-        <v>0.0327511839750556</v>
+        <v>0.0322210589943279</v>
       </c>
       <c r="D49" t="n">
-        <v>-1.70541742603024</v>
+        <v>-1.98669709903951</v>
       </c>
       <c r="E49" t="n">
-        <v>0.111688483082496</v>
+        <v>0.0684149724450464</v>
       </c>
       <c r="F49" t="n">
-        <v>-0.0401450525542095</v>
+        <v>-0.0438193653399708</v>
       </c>
       <c r="G49" t="n">
-        <v>0.0372502157213898</v>
+        <v>0.0360248628524821</v>
       </c>
       <c r="H49" t="n">
-        <v>-1.07771329042686</v>
+        <v>-1.21636452911442</v>
       </c>
       <c r="I49" t="n">
-        <v>0.300723415511703</v>
+        <v>0.245537954000451</v>
       </c>
       <c r="J49"/>
       <c r="K49"/>
@@ -3480,28 +3480,28 @@
         <v>73</v>
       </c>
       <c r="B50" t="n">
-        <v>-0.0094375777558045</v>
+        <v>-0.00817206272152688</v>
       </c>
       <c r="C50" t="n">
-        <v>0.00818616280856667</v>
+        <v>0.00836498768303424</v>
       </c>
       <c r="D50" t="n">
-        <v>-1.15286954052859</v>
+        <v>-0.976936611407253</v>
       </c>
       <c r="E50" t="n">
-        <v>0.275432965435765</v>
+        <v>0.351227131636987</v>
       </c>
       <c r="F50" t="n">
-        <v>-0.00580946652862478</v>
+        <v>-0.00538797022599707</v>
       </c>
       <c r="G50" t="n">
-        <v>0.00961053585714539</v>
+        <v>0.00954431092751993</v>
       </c>
       <c r="H50" t="n">
-        <v>-0.604489345337125</v>
+        <v>-0.564521657656968</v>
       </c>
       <c r="I50" t="n">
-        <v>0.560066043592473</v>
+        <v>0.585848806700591</v>
       </c>
       <c r="J50"/>
       <c r="K50"/>
@@ -3525,28 +3525,28 @@
         <v>74</v>
       </c>
       <c r="B51" t="n">
-        <v>-0.00650739959325846</v>
+        <v>-0.00690041306667753</v>
       </c>
       <c r="C51" t="n">
-        <v>0.00627917071360293</v>
+        <v>0.00635940581295514</v>
       </c>
       <c r="D51" t="n">
-        <v>-1.03634697797929</v>
+        <v>-1.08507198150813</v>
       </c>
       <c r="E51" t="n">
-        <v>0.317283740144828</v>
+        <v>0.295866955419126</v>
       </c>
       <c r="F51" t="n">
-        <v>-0.00544986700874848</v>
+        <v>-0.00542360158020943</v>
       </c>
       <c r="G51" t="n">
-        <v>0.00813079575365101</v>
+        <v>0.00814992630349973</v>
       </c>
       <c r="H51" t="n">
-        <v>-0.670274739874175</v>
+        <v>-0.66547860412927</v>
       </c>
       <c r="I51" t="n">
-        <v>0.513694205615087</v>
+        <v>0.516681849659811</v>
       </c>
       <c r="J51"/>
       <c r="K51"/>
@@ -3570,28 +3570,28 @@
         <v>75</v>
       </c>
       <c r="B52" t="n">
-        <v>-0.00116589528642682</v>
+        <v>-0.00106234175242482</v>
       </c>
       <c r="C52" t="n">
-        <v>0.0019968137385002</v>
+        <v>0.00179622459937777</v>
       </c>
       <c r="D52" t="n">
-        <v>-0.58387783694964</v>
+        <v>-0.591430354974998</v>
       </c>
       <c r="E52" t="n">
-        <v>0.656814562241999</v>
+        <v>0.653298002787607</v>
       </c>
       <c r="F52" t="n">
-        <v>-0.000430047335081728</v>
+        <v>-0.000417854039995796</v>
       </c>
       <c r="G52" t="n">
-        <v>0.00585601964344127</v>
+        <v>0.00595363929808808</v>
       </c>
       <c r="H52" t="n">
-        <v>-0.0734367985878223</v>
+        <v>-0.0701846415401725</v>
       </c>
       <c r="I52" t="n">
-        <v>0.952568610715684</v>
+        <v>0.954662062889325</v>
       </c>
       <c r="J52"/>
       <c r="K52"/>
@@ -3615,28 +3615,28 @@
         <v>76</v>
       </c>
       <c r="B53" t="n">
-        <v>0.0191167566148813</v>
+        <v>0.0189365312842562</v>
       </c>
       <c r="C53" t="n">
-        <v>0.0131266164539044</v>
+        <v>0.0127485093235105</v>
       </c>
       <c r="D53" t="n">
-        <v>1.45633542977446</v>
+        <v>1.48539180571754</v>
       </c>
       <c r="E53" t="n">
-        <v>0.170439266304362</v>
+        <v>0.163016135050472</v>
       </c>
       <c r="F53" t="n">
-        <v>0.0247995775558236</v>
+        <v>0.0236583417073779</v>
       </c>
       <c r="G53" t="n">
-        <v>0.0146847566564654</v>
+        <v>0.0145084880720696</v>
       </c>
       <c r="H53" t="n">
-        <v>1.68879731111546</v>
+        <v>1.63065521299375</v>
       </c>
       <c r="I53" t="n">
-        <v>0.116239165457507</v>
+        <v>0.128027895384474</v>
       </c>
       <c r="J53"/>
       <c r="K53"/>
@@ -3660,28 +3660,28 @@
         <v>77</v>
       </c>
       <c r="B54" t="n">
-        <v>0.00801632557669242</v>
+        <v>0.00832173810374132</v>
       </c>
       <c r="C54" t="n">
-        <v>0.0135234803747961</v>
+        <v>0.0118888728204018</v>
       </c>
       <c r="D54" t="n">
-        <v>0.592770895843688</v>
+        <v>0.69996022578868</v>
       </c>
       <c r="E54" t="n">
-        <v>0.562231564521265</v>
+        <v>0.494754727146166</v>
       </c>
       <c r="F54" t="n">
-        <v>0.0140840729018088</v>
+        <v>0.0150253378715686</v>
       </c>
       <c r="G54" t="n">
-        <v>0.0167096371880071</v>
+        <v>0.0166926066641254</v>
       </c>
       <c r="H54" t="n">
-        <v>0.842871257068182</v>
+        <v>0.900119326711267</v>
       </c>
       <c r="I54" t="n">
-        <v>0.412547541633177</v>
+        <v>0.382267382773602</v>
       </c>
       <c r="J54"/>
       <c r="K54"/>
@@ -3705,28 +3705,28 @@
         <v>78</v>
       </c>
       <c r="B55" t="n">
-        <v>0.00000411159421524973</v>
+        <v>0.00000471245923539559</v>
       </c>
       <c r="C55" t="n">
-        <v>0.00000533992071850374</v>
+        <v>0.00000540679246780462</v>
       </c>
       <c r="D55" t="n">
-        <v>0.769972895103546</v>
+        <v>0.871581305081798</v>
       </c>
       <c r="E55" t="n">
-        <v>0.456585991116922</v>
+        <v>0.400866892700173</v>
       </c>
       <c r="F55" t="n">
-        <v>0.00000473472439487353</v>
+        <v>0.00000459966488250379</v>
       </c>
       <c r="G55" t="n">
-        <v>0.0000064277675860604</v>
+        <v>0.00000643544614575535</v>
       </c>
       <c r="H55" t="n">
-        <v>0.736604790307214</v>
+        <v>0.71473908386874</v>
       </c>
       <c r="I55" t="n">
-        <v>0.4770087906543</v>
+        <v>0.489896248320798</v>
       </c>
       <c r="J55"/>
       <c r="K55"/>
@@ -3750,28 +3750,28 @@
         <v>79</v>
       </c>
       <c r="B56" t="n">
-        <v>0.000012990245560264</v>
+        <v>0.0000131744971371344</v>
       </c>
       <c r="C56" t="n">
-        <v>0.00000261329171383262</v>
+        <v>0.00000270446352139403</v>
       </c>
       <c r="D56" t="n">
-        <v>4.97083639438504</v>
+        <v>4.87139021581017</v>
       </c>
       <c r="E56" t="n">
-        <v>0.000157574352663973</v>
+        <v>0.000190546743892024</v>
       </c>
       <c r="F56" t="n">
-        <v>0.0000146112674640579</v>
+        <v>0.0000146428642860518</v>
       </c>
       <c r="G56" t="n">
-        <v>0.00000354359376494372</v>
+        <v>0.00000355909894031179</v>
       </c>
       <c r="H56" t="n">
-        <v>4.12329077012302</v>
+        <v>4.11420545807278</v>
       </c>
       <c r="I56" t="n">
-        <v>0.0010271045795707</v>
+        <v>0.0010463479798236</v>
       </c>
       <c r="J56"/>
       <c r="K56"/>
@@ -3795,16 +3795,16 @@
         <v>80</v>
       </c>
       <c r="B57" t="n">
-        <v>-0.520624204390131</v>
+        <v>-0.420378765862341</v>
       </c>
       <c r="C57" t="n">
-        <v>0.255858907673384</v>
+        <v>0.147151077353121</v>
       </c>
       <c r="D57" t="n">
-        <v>-2.03480976732197</v>
+        <v>-2.85678347331124</v>
       </c>
       <c r="E57" t="n">
-        <v>0.0714164074421516</v>
+        <v>0.0248218596528998</v>
       </c>
       <c r="F57"/>
       <c r="G57"/>
@@ -3832,16 +3832,16 @@
         <v>81</v>
       </c>
       <c r="B58" t="n">
-        <v>-0.212087386398799</v>
+        <v>-0.143513321031857</v>
       </c>
       <c r="C58" t="n">
-        <v>0.0583554720460172</v>
+        <v>0.0591640895792885</v>
       </c>
       <c r="D58" t="n">
-        <v>-3.63440443479839</v>
+        <v>-2.4256829109071</v>
       </c>
       <c r="E58" t="n">
-        <v>0.00281015665807479</v>
+        <v>0.0307397061412903</v>
       </c>
       <c r="F58"/>
       <c r="G58"/>
@@ -3869,16 +3869,16 @@
         <v>82</v>
       </c>
       <c r="B59" t="n">
-        <v>-0.367078578977402</v>
+        <v>-0.358078047711752</v>
       </c>
       <c r="C59" t="n">
-        <v>0.128504548157309</v>
+        <v>0.139982762077844</v>
       </c>
       <c r="D59" t="n">
-        <v>-2.85654153289611</v>
+        <v>-2.55801530414599</v>
       </c>
       <c r="E59" t="n">
-        <v>0.0131036813062166</v>
+        <v>0.0227796313697603</v>
       </c>
       <c r="F59"/>
       <c r="G59"/>
@@ -3906,16 +3906,16 @@
         <v>83</v>
       </c>
       <c r="B60" t="n">
-        <v>0.258047637442117</v>
+        <v>0.275181586299913</v>
       </c>
       <c r="C60" t="n">
-        <v>0.0768211746425154</v>
+        <v>0.0835222493833118</v>
       </c>
       <c r="D60" t="n">
-        <v>3.35906914523154</v>
+        <v>3.2947099525183</v>
       </c>
       <c r="E60" t="n">
-        <v>0.0040101460346859</v>
+        <v>0.0047630973141477</v>
       </c>
       <c r="F60"/>
       <c r="G60"/>
@@ -3943,16 +3943,16 @@
         <v>84</v>
       </c>
       <c r="B61" t="n">
-        <v>-0.622816499678336</v>
+        <v>-0.668024106239868</v>
       </c>
       <c r="C61" t="n">
-        <v>0.102690993628213</v>
+        <v>0.0908035614610111</v>
       </c>
       <c r="D61" t="n">
-        <v>-6.06495738013025</v>
+        <v>-7.35680512406666</v>
       </c>
       <c r="E61" t="n">
-        <v>0.000331465487056523</v>
+        <v>0.000115112230119864</v>
       </c>
       <c r="F61"/>
       <c r="G61"/>

</xml_diff>